<commit_message>
Aanvullen van de tijdsbesteding
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>week 12-18/10/2015</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>totaal:</t>
+  </si>
+  <si>
+    <t>gemiddeld:</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -489,6 +492,13 @@
       <c r="B3" s="3">
         <v>22</v>
       </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="4">
+        <f>AVERAGE(B2:B8)</f>
+        <v>18.5</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
@@ -523,7 +533,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
-    <ignoredError sqref="E2" emptyCellReference="1"/>
+    <ignoredError sqref="E2:E3" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Toevoegen van de tijdsbesteding op maandag 19/10/2015
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="h\.mm&quot; u.&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="h\.mm&quot; u.&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,7 +115,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -497,14 +497,16 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>18.5</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">

</xml_diff>

<commit_message>
Update van de tijdsbestedingen
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>13.333333333333334</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -505,14 +505,18 @@
         <v>1</v>
       </c>
       <c r="B4" s="3">
-        <v>3</v>
+        <f>5+2+5</f>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
+      <c r="B5" s="3">
+        <f>5</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
update van de tijdsbesteding
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="2580" yWindow="660" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>13.5</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -514,15 +514,18 @@
         <v>3</v>
       </c>
       <c r="B5" s="3">
-        <f>5</f>
-        <v>5</v>
+        <f>5+1</f>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="3">
+        <f>4</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">

</xml_diff>

<commit_message>
Update tijdsbestedingen na maandag
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -481,7 +481,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>11.8</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -523,8 +523,8 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f>4</f>
-        <v>4</v>
+        <f>7</f>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>

<commit_message>
Update van de tijdsbesteding: afgelopen 2 weken
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="660" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="660" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -59,8 +64,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="h\.mm&quot; u.&quot;;@"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="h\.mm&quot; u.&quot;;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -103,7 +108,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -111,18 +116,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normaal" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -451,17 +461,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -469,7 +479,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -481,11 +491,11 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>62</v>
+        <v>82.08</v>
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,10 +507,10 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>12.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>11.725714285714286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -509,7 +519,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -518,36 +528,37 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <f>7</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <f>7+1+1+0.5+3</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="B7" s="3">
+        <f>4.75+3.33+2.5</f>
+        <v>10.58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3">
+        <f>4</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <ignoredErrors>
     <ignoredError sqref="E2:E3" emptyCellReference="1"/>
   </ignoredErrors>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aanvulling voor week 16-22/11
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -461,7 +461,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,7 +491,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B8)</f>
-        <v>82.08</v>
+        <v>88.08</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -507,7 +507,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B8)</f>
-        <v>11.725714285714286</v>
+        <v>12.582857142857142</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -551,8 +551,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3">
-        <f>4</f>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aanvulling van week 23-29/11 + aanvullen van de data.
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>week 12-18/10/2015</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>gemiddeld:</t>
+  </si>
+  <si>
+    <t>week 23-29/11/2015</t>
+  </si>
+  <si>
+    <t>week 30-06/12/2015</t>
+  </si>
+  <si>
+    <t>week 07-13/12/2015</t>
+  </si>
+  <si>
+    <t>week 14-20/12/2015</t>
   </si>
 </sst>
 </file>
@@ -458,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,8 +502,8 @@
         <v>9</v>
       </c>
       <c r="E2" s="4">
-        <f>SUM(B2:B8)</f>
-        <v>88.08</v>
+        <f>SUM(B2:B12)</f>
+        <v>96.08</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -506,8 +518,8 @@
         <v>10</v>
       </c>
       <c r="E3" s="4">
-        <f>AVERAGE(B2:B8)</f>
-        <v>12.582857142857142</v>
+        <f>AVERAGE(B2:B12)</f>
+        <v>12.01</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -554,10 +566,34 @@
         <v>10</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3">
+        <f>5+1+2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ignoredErrors>
-    <ignoredError sqref="E2:E3" emptyCellReference="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added tijdsmetingen en tijdsbesteding
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="560" yWindow="660" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
+    <workbookView xWindow="555" yWindow="660" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -135,8 +130,8 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -473,17 +468,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -491,7 +486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -503,11 +498,11 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B12)</f>
-        <v>96.08</v>
+        <v>105.33</v>
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,10 +514,10 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B12)</f>
-        <v>12.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11.703333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -531,7 +526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -540,7 +535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -549,7 +544,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -558,7 +553,7 @@
         <v>10.58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -566,28 +561,30 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3">
-        <f>5+1+2</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <f>5+1+2+3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="3">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Update tijdsbesteding voor het 8e rapport
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -473,7 +473,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B12)</f>
-        <v>109.08</v>
+        <v>112.08</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B12)</f>
-        <v>12.12</v>
+        <v>11.208</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,7 +588,10 @@
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="3">
+        <f>3</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">

</xml_diff>

<commit_message>
Update van de tijdsbesteding voor week 7-13 en week 14-20
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +503,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B12)</f>
-        <v>112.08</v>
+        <v>133.57999999999998</v>
       </c>
       <c r="F2" s="5"/>
     </row>
@@ -519,7 +519,7 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B12)</f>
-        <v>11.208</v>
+        <v>12.143636363636363</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -589,15 +589,18 @@
         <v>13</v>
       </c>
       <c r="B11" s="3">
-        <f>3</f>
-        <v>3</v>
+        <f>3+6+7</f>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="3">
+        <f>5+3.5</f>
+        <v>8.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated representatie van netwerk (W) Updated tijdsbesteding Started 'brainstorming' on implementation w multiple threads.
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mathias/Desktop/WV_SortingNetworks/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -153,9 +148,9 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Komma" xfId="1" builtinId="3"/>
-    <cellStyle name="Procent" xfId="2" builtinId="5"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -492,17 +487,17 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -510,7 +505,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -522,7 +517,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B14)</f>
-        <v>153.07999999999998</v>
+        <v>165.07999999999998</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -534,7 +529,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,18 +541,18 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B14)</f>
-        <v>11.775384615384613</v>
+        <v>12.698461538461537</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>0.68035555555555549</v>
+        <v>0.73368888888888883</v>
       </c>
       <c r="H3" s="7">
         <f>E2/H2</f>
-        <v>0.56696296296296289</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.6114074074074074</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -566,7 +561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -575,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -584,7 +579,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -593,7 +588,7 @@
         <v>10.58</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -601,7 +596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -610,7 +605,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -619,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -628,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -637,21 +632,21 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="3">
-        <f>7.5</f>
-        <v>7.5</v>
+        <f>7.5+4+3</f>
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tijdsbesteding + meer test runs VSC
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>week 12-18/10/2015</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>week 15-21/02/2016</t>
+  </si>
+  <si>
+    <t>week 22-28/02/2016</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -529,7 +532,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B18)</f>
-        <v>189.07999999999998</v>
+        <v>198.07999999999998</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -553,15 +556,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B18)</f>
-        <v>12.605333333333332</v>
+        <v>12.379999999999999</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>0.84035555555555552</v>
+        <v>0.88035555555555545</v>
       </c>
       <c r="H3" s="7">
         <f>E2/H2</f>
-        <v>0.70029629629629619</v>
+        <v>0.73362962962962952</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -675,9 +678,21 @@
         <v>18</v>
       </c>
       <c r="B16" s="3">
-        <f xml:space="preserve"> 6 + 4</f>
-        <v>10</v>
-      </c>
+        <f xml:space="preserve"> 6 + 4 + 3</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="3">
+        <f xml:space="preserve"> 6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated some excel files
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>week 12-18/10/2015</t>
   </si>
@@ -99,6 +102,15 @@
   </si>
   <si>
     <t>week 28-03/04/2016</t>
+  </si>
+  <si>
+    <t>week 04-10/04/2016</t>
+  </si>
+  <si>
+    <t>week 11-17/04/2016</t>
+  </si>
+  <si>
+    <t>week 18-24/04/2016</t>
   </si>
 </sst>
 </file>
@@ -513,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +559,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B22)</f>
-        <v>231.57999999999998</v>
+        <v>243.57999999999998</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -571,15 +583,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B22)</f>
-        <v>12.188421052631577</v>
+        <v>11.599047619047619</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.0292444444444444</v>
+        <v>1.0825777777777776</v>
       </c>
       <c r="H3" s="7">
         <f>E2/H2</f>
-        <v>0.85770370370370363</v>
+        <v>0.90214814814814814</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,18 +741,40 @@
         <v>22</v>
       </c>
       <c r="B20" s="3">
-        <f xml:space="preserve"> 2 + 2.5</f>
-        <v>4.5</v>
+        <f xml:space="preserve"> 2 + 2.5 + 5</f>
+        <v>9.5</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="B22" s="3">
+        <f xml:space="preserve"> 5 + 2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added some bib, some tex and updated tijdsbesteding
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -172,7 +172,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -187,6 +187,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -528,7 +529,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,8 +559,8 @@
         <v>9</v>
       </c>
       <c r="E2" s="4">
-        <f>SUM(B2:B22)</f>
-        <v>243.57999999999998</v>
+        <f>SUM(B2:B25)</f>
+        <v>268.08</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -582,16 +583,16 @@
         <v>10</v>
       </c>
       <c r="E3" s="4">
-        <f>AVERAGE(B2:B22)</f>
-        <v>11.599047619047619</v>
+        <f>AVERAGE(B2:B25)</f>
+        <v>11.655652173913042</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.0825777777777776</v>
-      </c>
-      <c r="H3" s="7">
+        <v>1.1914666666666667</v>
+      </c>
+      <c r="H3" s="8">
         <f>E2/H2</f>
-        <v>0.90214814814814814</v>
+        <v>0.99288888888888882</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -750,7 +751,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -758,24 +759,32 @@
         <v>24</v>
       </c>
       <c r="B22" s="3">
-        <f xml:space="preserve"> 5 + 2</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B23" s="3">
+        <f xml:space="preserve"> 5 + 2 + 4</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B24" s="3">
+        <f xml:space="preserve"> 6 + 3 + 3.5</f>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update 05/05 - 19:30
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B29)</f>
-        <v>323.83</v>
+        <v>331.08</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -582,15 +582,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B29)</f>
-        <v>12.455</v>
+        <v>12.733846153846153</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.4392444444444443</v>
+        <v>1.4714666666666667</v>
       </c>
       <c r="H3" s="8">
         <f>E2/H2</f>
-        <v>1.1993703703703704</v>
+        <v>1.2262222222222221</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -801,8 +801,8 @@
         <v>29</v>
       </c>
       <c r="B27" s="3">
-        <f xml:space="preserve"> 4.5 + 4 + 1.5 + 1 + 2.5 + 1 + 1.5</f>
-        <v>16</v>
+        <f xml:space="preserve"> 4.5 + 4 + 1.5 + 1 + 2.5 + 1 + 1.5 + 2.5 + 3.25 + 1.5</f>
+        <v>23.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update voor 6/05 15:20
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -527,7 +527,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -558,7 +558,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B29)</f>
-        <v>333.58</v>
+        <v>334.58</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -582,15 +582,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B29)</f>
-        <v>12.83</v>
+        <v>12.868461538461538</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.4825777777777778</v>
+        <v>1.4870222222222222</v>
       </c>
       <c r="H3" s="8">
         <f>E2/H2</f>
-        <v>1.2354814814814814</v>
+        <v>1.2391851851851852</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -801,8 +801,8 @@
         <v>29</v>
       </c>
       <c r="B27" s="3">
-        <f xml:space="preserve"> 4.5 + 4 + 1.5 + 1 + 2.5 + 1 + 1.5 + 2.5 + 3.25 + 1.5 + 2.5</f>
-        <v>25.75</v>
+        <f xml:space="preserve"> 4.5 + 4 + 1.5 + 1 + 2.5 + 1 + 1.5 + 2.5 + 3.25 + 1.5 + 2.5 + 1</f>
+        <v>26.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update the tijdsbesteding file.
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>week 12-18/10/2015</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>week 09-15/05/2016</t>
+  </si>
+  <si>
+    <t>week 16-22/05/2016</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -561,7 +564,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B29)</f>
-        <v>342.08</v>
+        <v>352.08</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -585,15 +588,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B29)</f>
-        <v>12.669629629629629</v>
+        <v>12.574285714285713</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.5203555555555555</v>
+        <v>1.5648</v>
       </c>
       <c r="H3" s="8">
         <f>E2/H2</f>
-        <v>1.2669629629629628</v>
+        <v>1.304</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -815,6 +818,15 @@
       <c r="B28" s="3">
         <f xml:space="preserve"> 7.5</f>
         <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="3">
+        <f>6+2+2</f>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update tijdsbesteding - 20/05/2016 10u
</commit_message>
<xml_diff>
--- a/tijdsbesteding.xlsx
+++ b/tijdsbesteding.xlsx
@@ -533,7 +533,7 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -564,7 +564,7 @@
       </c>
       <c r="E2" s="4">
         <f>SUM(B2:B29)</f>
-        <v>352.08</v>
+        <v>353.08</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="1">
@@ -588,15 +588,15 @@
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(B2:B29)</f>
-        <v>12.574285714285713</v>
+        <v>12.61</v>
       </c>
       <c r="G3" s="7">
         <f>E2/G2</f>
-        <v>1.5648</v>
+        <v>1.5692444444444444</v>
       </c>
       <c r="H3" s="8">
         <f>E2/H2</f>
-        <v>1.304</v>
+        <v>1.3077037037037036</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -825,8 +825,8 @@
         <v>31</v>
       </c>
       <c r="B29" s="3">
-        <f>6+2+2</f>
-        <v>10</v>
+        <f>6+2+2+1</f>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>